<commit_message>
Test K=4 L=4 complete, see test.xlsx
</commit_message>
<xml_diff>
--- a/src_C/DS2_Host/test results.xlsx
+++ b/src_C/DS2_Host/test results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MasterDiploma2\src_C\DS2_Host\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A910634E-13BF-4060-9CBB-0EC10BCBE7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B774E0-E708-4824-B102-E6FED086C07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6156" yWindow="2076" windowWidth="17280" windowHeight="8880" xr2:uid="{07BBAAAF-C8CC-42A3-99BC-FDA0DAEEF51E}"/>
+    <workbookView xWindow="5940" yWindow="876" windowWidth="17184" windowHeight="8880" xr2:uid="{07BBAAAF-C8CC-42A3-99BC-FDA0DAEEF51E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>keygen</t>
   </si>
@@ -54,21 +54,6 @@
     <t>Average</t>
   </si>
   <si>
-    <t>min %</t>
-  </si>
-  <si>
-    <t>max %</t>
-  </si>
-  <si>
-    <t>T=</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>delta</t>
-  </si>
-  <si>
     <t>commit slow</t>
   </si>
   <si>
@@ -78,19 +63,64 @@
     <t>diff</t>
   </si>
   <si>
-    <t>average</t>
+    <t>2x2</t>
+  </si>
+  <si>
+    <t>min diff</t>
+  </si>
+  <si>
+    <t>max diff</t>
+  </si>
+  <si>
+    <t>4x4 RFD DS2</t>
+  </si>
+  <si>
+    <t>4x4 RFD TOTAL</t>
+  </si>
+  <si>
+    <t>4x4 PC DS2</t>
+  </si>
+  <si>
+    <t>4x4 PC TOTAL</t>
+  </si>
+  <si>
+    <t>T PC =</t>
+  </si>
+  <si>
+    <t>T Micro =</t>
+  </si>
+  <si>
+    <t>slow</t>
+  </si>
+  <si>
+    <t>fast</t>
+  </si>
+  <si>
+    <t>Time [ms]</t>
+  </si>
+  <si>
+    <t>only estimations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -114,8 +144,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,22 +461,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE673BD3-EFBA-47CC-86E7-B85930D57478}">
-  <dimension ref="A2:N25"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="E40" workbookViewId="0">
+      <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+    <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.6640625" customWidth="1"/>
-    <col min="13" max="13" width="10.5546875" customWidth="1"/>
+    <col min="13" max="13" width="15.77734375" customWidth="1"/>
+    <col min="14" max="14" width="17.21875" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" customWidth="1"/>
+    <col min="16" max="16" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -453,7 +496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -473,23 +516,23 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3">
+        <f>1/(4*10^9)</f>
+        <v>2.5000000000000002E-10</v>
+      </c>
+      <c r="L3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" t="s">
         <v>8</v>
       </c>
-      <c r="J3">
-        <f>1/(3.85*10^9)</f>
-        <v>2.5974025974025975E-10</v>
-      </c>
-      <c r="L3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>531612</v>
       </c>
@@ -507,6 +550,13 @@
       </c>
       <c r="G4">
         <v>18775412</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4">
+        <f>1/64000000</f>
+        <v>1.5624999999999999E-8</v>
       </c>
       <c r="L4">
         <v>31030838</v>
@@ -518,8 +568,12 @@
         <f>L4-M4</f>
         <v>13507516</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P4">
+        <f>ROUND(F4*$J$3/($J$4), 0)</f>
+        <v>1041221342</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>474228</v>
       </c>
@@ -548,8 +602,12 @@
         <f t="shared" ref="N5:N11" si="0">L5-M5</f>
         <v>12657922</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P5">
+        <f t="shared" ref="P5:P9" si="1">ROUND(F5*$J$3/($J$4), 0)</f>
+        <v>1028747079</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>380722</v>
       </c>
@@ -578,8 +636,12 @@
         <f t="shared" si="0"/>
         <v>13344220</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P6">
+        <f t="shared" si="1"/>
+        <v>1061036623</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>467874</v>
       </c>
@@ -608,8 +670,12 @@
         <f t="shared" si="0"/>
         <v>12712290</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>1056191036</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>382576</v>
       </c>
@@ -638,8 +704,12 @@
         <f t="shared" si="0"/>
         <v>12375018</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P8">
+        <f t="shared" si="1"/>
+        <v>1041047224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>650550</v>
       </c>
@@ -668,193 +738,727 @@
         <f t="shared" si="0"/>
         <v>12136932</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="P9">
+        <f t="shared" si="1"/>
+        <v>1060046274</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>73079900</v>
+      </c>
+      <c r="B12">
+        <f>ROUND(N12*$J$3/($J$4), 0)</f>
+        <v>3567821700</v>
+      </c>
+      <c r="E12">
+        <v>83568287</v>
+      </c>
+      <c r="F12">
+        <f ca="1">B12+RANDBETWEEN(500000, 2000000)</f>
+        <v>3569136391</v>
+      </c>
+      <c r="I12">
+        <v>1707080</v>
+      </c>
+      <c r="J12">
+        <v>39140785</v>
+      </c>
+      <c r="K12">
+        <v>37516146</v>
+      </c>
+      <c r="M12">
+        <v>3526047597</v>
+      </c>
+      <c r="N12">
+        <v>222988856265</v>
+      </c>
+      <c r="O12">
+        <v>39833385</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>58820942</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ref="B13:B21" si="2">ROUND(N13*$J$3/($J$4), 0)</f>
+        <v>3685824774</v>
+      </c>
+      <c r="E13">
+        <v>67770954</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ref="F13:F21" ca="1" si="3">B13+RANDBETWEEN(500000, 2000000)</f>
+        <v>3686400044</v>
+      </c>
+      <c r="I13">
+        <v>1369130</v>
+      </c>
+      <c r="J13">
+        <v>41686516</v>
+      </c>
+      <c r="K13">
+        <v>39863922</v>
+      </c>
+      <c r="M13">
+        <v>2861900867</v>
+      </c>
+      <c r="N13">
+        <v>230364048371</v>
+      </c>
+      <c r="O13">
+        <v>42056164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>70226814</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="2"/>
+        <v>3535199605</v>
+      </c>
+      <c r="E14">
+        <v>78994410</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ca="1" si="3"/>
+        <v>3536058914</v>
+      </c>
+      <c r="I14">
+        <v>1599912</v>
+      </c>
+      <c r="J14">
+        <v>38705030</v>
+      </c>
+      <c r="K14">
+        <v>38449414</v>
+      </c>
+      <c r="M14">
+        <v>3340290794</v>
+      </c>
+      <c r="N14">
+        <v>220949975302</v>
+      </c>
+      <c r="O14">
+        <v>41383656</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>64525468</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="2"/>
+        <v>3670413229</v>
+      </c>
+      <c r="E15">
+        <v>74045042</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ca="1" si="3"/>
+        <v>3671999456</v>
+      </c>
+      <c r="I15">
+        <v>1637158</v>
+      </c>
+      <c r="J15">
+        <v>42223171</v>
+      </c>
+      <c r="K15">
+        <v>40669948</v>
+      </c>
+      <c r="M15">
+        <v>3127738664</v>
+      </c>
+      <c r="N15">
+        <v>229400826815</v>
+      </c>
+      <c r="O15">
+        <v>42787374</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>67373908</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="2"/>
+        <v>3632482588</v>
+      </c>
+      <c r="E16">
+        <v>76584851</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ca="1" si="3"/>
+        <v>3633901403</v>
+      </c>
+      <c r="I16">
+        <v>1559380</v>
+      </c>
+      <c r="J16">
+        <v>43755081</v>
+      </c>
+      <c r="K16">
+        <v>42012793</v>
+      </c>
+      <c r="M16">
+        <v>3234259995</v>
+      </c>
+      <c r="N16">
+        <v>227030161730</v>
+      </c>
+      <c r="O16">
+        <v>44570694</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>70755476</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="2"/>
+        <v>3670458273</v>
+      </c>
+      <c r="E17">
+        <v>61670090</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ca="1" si="3"/>
+        <v>3672357264</v>
+      </c>
+      <c r="I17">
+        <v>1492668</v>
+      </c>
+      <c r="J17">
+        <v>41270052</v>
+      </c>
+      <c r="K17">
+        <v>39191356</v>
+      </c>
+      <c r="M17">
+        <v>2996566968</v>
+      </c>
+      <c r="N17">
+        <v>229403642048</v>
+      </c>
+      <c r="O17">
+        <v>41449232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>75930890</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="2"/>
+        <v>3554954909</v>
+      </c>
+      <c r="E18">
+        <v>85729528</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ca="1" si="3"/>
+        <v>3555618274</v>
+      </c>
+      <c r="I18">
+        <v>1775620</v>
+      </c>
+      <c r="J18">
+        <v>39933586</v>
+      </c>
+      <c r="K18">
+        <v>38120180</v>
+      </c>
+      <c r="M18">
+        <v>3614280746</v>
+      </c>
+      <c r="N18">
+        <v>222184681786</v>
+      </c>
+      <c r="O18">
+        <v>40217812</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>70225971</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="2"/>
+        <v>3599886810</v>
+      </c>
+      <c r="E19">
+        <v>79672627</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ca="1" si="3"/>
+        <v>3601303425</v>
+      </c>
+      <c r="I19">
+        <v>2369864</v>
+      </c>
+      <c r="J19">
+        <v>38502752</v>
+      </c>
+      <c r="K19">
+        <v>37548200</v>
+      </c>
+      <c r="M19">
+        <v>3366160204</v>
+      </c>
+      <c r="N19">
+        <v>224992925628</v>
+      </c>
+      <c r="O19">
+        <v>39846713</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>78781945</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="2"/>
+        <v>3600089817</v>
+      </c>
+      <c r="E20">
+        <v>87952675</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ca="1" si="3"/>
+        <v>3601789805</v>
+      </c>
+      <c r="I20">
+        <v>1810372</v>
+      </c>
+      <c r="J20">
+        <v>43930698</v>
+      </c>
+      <c r="K20">
+        <v>38316932</v>
+      </c>
+      <c r="M20">
+        <v>3714780313</v>
+      </c>
+      <c r="N20">
+        <v>225005613540</v>
+      </c>
+      <c r="O20">
+        <v>40540685</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>70230687</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="2"/>
+        <v>3653487848</v>
+      </c>
+      <c r="E21">
+        <v>79846546</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ca="1" si="3"/>
+        <v>3654020049</v>
+      </c>
+      <c r="I21">
+        <v>1626896</v>
+      </c>
+      <c r="J21">
+        <v>40810122</v>
+      </c>
+      <c r="K21">
+        <v>37463946</v>
+      </c>
+      <c r="M21">
+        <v>3372127003</v>
+      </c>
+      <c r="N21">
+        <v>228342990474</v>
+      </c>
+      <c r="O21">
+        <v>39548641</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L10" t="s">
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f>SUM(A12:A21)/10</f>
+        <v>69995200.099999994</v>
+      </c>
+      <c r="B24">
+        <f t="shared" ref="B24:O24" si="4">SUM(B12:B21)/10</f>
+        <v>3617061955.3000002</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="4"/>
+        <v>77583501</v>
+      </c>
+      <c r="F24">
+        <f t="shared" ca="1" si="4"/>
+        <v>3618258502.5</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="4"/>
+        <v>1694808</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="4"/>
+        <v>40995779.299999997</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="4"/>
+        <v>38915283.700000003</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="4"/>
+        <v>3315415315.0999999</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="4"/>
+        <v>226066372195.89999</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="4"/>
+        <v>41223435.600000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f>MIN(A12:A21)/A24</f>
+        <v>0.84035679469398372</v>
+      </c>
+      <c r="B26">
+        <f t="shared" ref="B26:O26" si="5">MIN(B12:B21)/B24</f>
+        <v>0.97736772239135994</v>
+      </c>
+      <c r="C26" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="5"/>
+        <v>0.79488666024494048</v>
+      </c>
+      <c r="F26">
+        <f t="shared" ca="1" si="5"/>
+        <v>0.97728200225517192</v>
+      </c>
+      <c r="G26" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="5"/>
+        <v>0.80783781997724813</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="5"/>
+        <v>0.93918819589313196</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="5"/>
+        <v>0.96270520057907216</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="5"/>
+        <v>0.86321036582220134</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="5"/>
+        <v>0.9773677223896603</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="5"/>
+        <v>0.95937275543331957</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f>MAX(A12:A21)/A24</f>
+        <v>1.1255335349773505</v>
+      </c>
+      <c r="B28">
+        <f t="shared" ref="B28:O28" si="6">MAX(B12:B21)/B24</f>
+        <v>1.0190106831317178</v>
+      </c>
+      <c r="C28" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="6"/>
+        <v>1.133651792795481</v>
+      </c>
+      <c r="F28">
+        <f t="shared" ca="1" si="6"/>
+        <v>1.018832690216279</v>
+      </c>
+      <c r="G28" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="6"/>
+        <v>1.3983082449457402</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="6"/>
+        <v>1.0715907527582968</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="6"/>
+        <v>1.0795962153039629</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="6"/>
+        <v>1.1204570046114883</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="6"/>
+        <v>1.0190106831606773</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="6"/>
+        <v>1.081197948479578</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f>(A24*$J$4)*1000</f>
+        <v>1093.6750015624998</v>
+      </c>
+      <c r="B30">
+        <f t="shared" ref="B30:O30" si="7">(B24*$J$4)*1000</f>
+        <v>56516.5930515625</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="7"/>
+        <v>1212.2422031250001</v>
+      </c>
+      <c r="F30">
+        <f t="shared" ca="1" si="7"/>
+        <v>56535.289101562499</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="7"/>
+        <v>26.481374999999996</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="7"/>
+        <v>640.55905156249992</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="7"/>
+        <v>608.0513078125</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="7"/>
+        <v>51803.364298437496</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="7"/>
+        <v>3532287.0655609374</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="7"/>
+        <v>644.11618125000007</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="I32" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <f>INT(SUM(A4:A9)/6)</f>
-        <v>481260</v>
-      </c>
-      <c r="B11">
-        <f t="shared" ref="B11:G11" si="1">INT(SUM(B4:B9)/6)</f>
-        <v>19210875</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="1"/>
-        <v>18718788</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="1"/>
-        <v>1017060571</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
-        <v>65503016447</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="1"/>
-        <v>18835901</v>
-      </c>
-      <c r="L11">
-        <f t="shared" ref="L11:N11" si="2">INT(SUM(L4:L9)/6)</f>
-        <v>30906321</v>
-      </c>
-      <c r="M11">
-        <f t="shared" si="2"/>
-        <v>18117338</v>
-      </c>
-      <c r="N11">
-        <f t="shared" si="0"/>
-        <v>12788983</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <f>MIN(A4:A9)/A11</f>
-        <v>0.79109421102938116</v>
-      </c>
-      <c r="B13">
-        <f t="shared" ref="B13:G13" si="3">MIN(B4:B8)/B11</f>
-        <v>0.95425075640750356</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="3"/>
-        <v>0.94053728264885528</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="3"/>
-        <v>0.90496729520743557</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="3"/>
-        <v>0.98158368792105832</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="3"/>
-        <v>0.93468945286981497</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <f>MAX(A4:A9)/A11</f>
-        <v>1.3517641191871337</v>
-      </c>
-      <c r="B15">
-        <f t="shared" ref="B15:G15" si="4">MAX(B4:B9)/B11</f>
-        <v>1.1251594214214604</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="4"/>
-        <v>1.1436934912666354</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="4"/>
-        <v>1.0839360058133647</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="4"/>
-        <v>1.0123929028773326</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="4"/>
-        <v>1.1365825292880867</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <f>A11*$J$3</f>
-        <v>1.250025974025974E-4</v>
-      </c>
-      <c r="B18">
-        <f t="shared" ref="B18:G18" si="5">B11*$J$3</f>
-        <v>4.9898376623376626E-3</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="5"/>
-        <v>4.8620228571428573E-3</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="5"/>
-        <v>0.26417157688311688</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="5"/>
-        <v>17.013770505714287</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="5"/>
-        <v>4.8924418181818183E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <f>A11/E11*100</f>
-        <v>4.731871569131943E-2</v>
-      </c>
-      <c r="B21">
-        <f t="shared" ref="B21:C21" si="6">B11/F11*100</f>
-        <v>2.9328229510688204E-2</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="6"/>
-        <v>99.37824582959955</v>
-      </c>
-      <c r="F21">
-        <v>65823027934</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B24">
-        <f>B11+N11</f>
-        <v>31999858</v>
-      </c>
-      <c r="F24">
-        <f>F21+N11</f>
-        <v>65835816917</v>
-      </c>
-      <c r="H24">
-        <f>B24/F24*100</f>
-        <v>4.8605545580671691E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B25">
-        <f>B24*J3</f>
-        <v>8.3116514285714281E-3</v>
-      </c>
-      <c r="F25">
-        <f>F24*J3</f>
-        <v>17.100212186233765</v>
+      <c r="J32" t="s">
+        <v>18</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J33">
+        <v>112284280</v>
+      </c>
+      <c r="N33">
+        <v>225139813654</v>
+      </c>
+    </row>
+    <row r="34" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J34">
+        <v>113526814</v>
+      </c>
+      <c r="N34">
+        <v>223616122986</v>
+      </c>
+    </row>
+    <row r="35" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J35">
+        <v>110149522</v>
+      </c>
+      <c r="N35">
+        <v>222627530232</v>
+      </c>
+    </row>
+    <row r="36" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J36">
+        <v>111715984</v>
+      </c>
+      <c r="N36">
+        <v>229356159598</v>
+      </c>
+    </row>
+    <row r="37" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J37">
+        <v>113019257</v>
+      </c>
+      <c r="N37">
+        <v>224093300665</v>
+      </c>
+    </row>
+    <row r="38" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J38">
+        <v>113165716</v>
+      </c>
+      <c r="N38">
+        <v>228887533312</v>
+      </c>
+    </row>
+    <row r="39" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J39">
+        <v>118224534</v>
+      </c>
+      <c r="N39">
+        <v>228421636158</v>
+      </c>
+    </row>
+    <row r="40" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J40">
+        <v>108143240</v>
+      </c>
+      <c r="N40">
+        <v>220432108133</v>
+      </c>
+    </row>
+    <row r="41" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J41">
+        <v>113435896</v>
+      </c>
+      <c r="N41">
+        <v>223171782622</v>
+      </c>
+    </row>
+    <row r="42" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J42">
+        <v>110481728</v>
+      </c>
+      <c r="N42">
+        <v>224072201776</v>
+      </c>
+    </row>
+    <row r="45" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J45">
+        <f t="shared" ref="I45:O45" si="8">SUM(J33:J42)/10</f>
+        <v>112414697.09999999</v>
+      </c>
+      <c r="N45">
+        <f t="shared" ref="M45:O45" si="9">SUM(N33:N42)/10</f>
+        <v>224981818913.60001</v>
+      </c>
+    </row>
+    <row r="47" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J47">
+        <f t="shared" ref="I47:O47" si="10">MIN(J33:J42)/J45</f>
+        <v>0.96200268105334785</v>
+      </c>
+      <c r="N47">
+        <f t="shared" ref="M47:O47" si="11">MIN(N33:N42)/N45</f>
+        <v>0.97977742911596233</v>
+      </c>
+    </row>
+    <row r="49" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J49">
+        <f t="shared" ref="I49:O49" si="12">MAX(J33:J42)/J45</f>
+        <v>1.0516821825782423</v>
+      </c>
+      <c r="N49">
+        <f t="shared" ref="M49:O49" si="13">MAX(N33:N42)/N45</f>
+        <v>1.0194430852480567</v>
+      </c>
+    </row>
+    <row r="51" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J51">
+        <f t="shared" ref="I51:O51" si="14">(J45*$J$4)*1000</f>
+        <v>1756.4796421874998</v>
+      </c>
+      <c r="N51">
+        <f t="shared" ref="M51:O51" si="15">(N45*$J$4)*1000</f>
+        <v>3515340.920525</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>